<commit_message>
committing the executed changes in configuration.properties, base class and test data.
</commit_message>
<xml_diff>
--- a/com.supermarket/src/main/resources/excelFile/TestData.xlsx
+++ b/com.supermarket/src/main/resources/excelFile/TestData.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="63">
   <si>
     <t>username</t>
   </si>
@@ -20,6 +20,9 @@
   </si>
   <si>
     <t>admin</t>
+  </si>
+  <si>
+    <t>admin123</t>
   </si>
   <si>
     <t>name</t>
@@ -522,7 +525,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -579,10 +582,10 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -611,10 +614,10 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -643,7 +646,7 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B6" s="1">
         <v>7.892134567E9</v>
@@ -675,10 +678,10 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -710,7 +713,7 @@
         <v>0</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -742,7 +745,7 @@
         <v>1</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -771,10 +774,10 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -803,10 +806,10 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -835,10 +838,10 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -867,10 +870,10 @@
     </row>
     <row r="13">
       <c r="A13" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -899,10 +902,10 @@
     </row>
     <row r="14">
       <c r="A14" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -931,10 +934,10 @@
     </row>
     <row r="15">
       <c r="A15" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -963,10 +966,10 @@
     </row>
     <row r="16">
       <c r="A16" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -995,10 +998,10 @@
     </row>
     <row r="17">
       <c r="A17" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -1027,10 +1030,10 @@
     </row>
     <row r="18">
       <c r="A18" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
@@ -1059,10 +1062,10 @@
     </row>
     <row r="19">
       <c r="A19" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
@@ -1091,10 +1094,10 @@
     </row>
     <row r="20">
       <c r="A20" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
@@ -1123,10 +1126,10 @@
     </row>
     <row r="21">
       <c r="A21" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -1155,7 +1158,7 @@
     </row>
     <row r="22">
       <c r="A22" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B22" s="4">
         <v>200.0</v>
@@ -1187,7 +1190,7 @@
     </row>
     <row r="23">
       <c r="A23" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B23" s="4">
         <v>100.0</v>
@@ -1219,7 +1222,7 @@
     </row>
     <row r="24">
       <c r="A24" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B24" s="4">
         <v>150.0</v>
@@ -1251,10 +1254,10 @@
     </row>
     <row r="25">
       <c r="A25" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
@@ -1283,7 +1286,7 @@
     </row>
     <row r="26">
       <c r="A26" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B26" s="4">
         <v>500.0</v>
@@ -1315,10 +1318,10 @@
     </row>
     <row r="27">
       <c r="A27" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
@@ -1347,10 +1350,10 @@
     </row>
     <row r="28">
       <c r="A28" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
@@ -1379,7 +1382,7 @@
     </row>
     <row r="29">
       <c r="A29" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B29" s="4">
         <v>925.0</v>
@@ -1411,10 +1414,10 @@
     </row>
     <row r="30">
       <c r="A30" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
@@ -1443,10 +1446,10 @@
     </row>
     <row r="31">
       <c r="A31" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
@@ -1475,7 +1478,7 @@
     </row>
     <row r="32">
       <c r="A32" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B32" s="6">
         <v>9.847556633E9</v>
@@ -1507,10 +1510,10 @@
     </row>
     <row r="33">
       <c r="A33" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
@@ -1539,7 +1542,7 @@
     </row>
     <row r="34">
       <c r="A34" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B34" s="7">
         <v>2010.0</v>
@@ -1571,10 +1574,10 @@
     </row>
     <row r="35">
       <c r="A35" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
@@ -1603,7 +1606,7 @@
     </row>
     <row r="36">
       <c r="A36" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B36" s="7">
         <v>1005.0</v>
@@ -1635,7 +1638,7 @@
     </row>
     <row r="37">
       <c r="A37" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B37" s="4">
         <v>145.0</v>
@@ -1667,10 +1670,10 @@
     </row>
     <row r="38">
       <c r="A38" s="7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
@@ -1697,7 +1700,7 @@
     </row>
     <row r="39">
       <c r="A39" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B39" s="9">
         <v>0.2</v>
@@ -1729,10 +1732,10 @@
     </row>
     <row r="40">
       <c r="A40" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
@@ -1761,10 +1764,10 @@
     </row>
     <row r="41">
       <c r="A41" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
@@ -1793,7 +1796,7 @@
     </row>
     <row r="42">
       <c r="A42" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B42" s="4">
         <v>200.0</v>
@@ -1825,7 +1828,7 @@
     </row>
     <row r="43">
       <c r="A43" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B43" s="9">
         <v>0.03</v>
@@ -1857,7 +1860,7 @@
     </row>
     <row r="44">
       <c r="A44" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B44" s="4">
         <v>100.0</v>
@@ -1889,10 +1892,10 @@
     </row>
     <row r="45">
       <c r="A45" s="4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
@@ -1924,7 +1927,7 @@
         <v>0</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
@@ -1956,7 +1959,7 @@
         <v>1</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
@@ -1985,7 +1988,7 @@
     </row>
     <row r="48">
       <c r="A48" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B48" s="1">
         <v>325.0</v>
@@ -2017,10 +2020,10 @@
     </row>
     <row r="49">
       <c r="A49" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>

</xml_diff>